<commit_message>
cleaning up the repo and getting rid of the 20 different versions of the diet code
</commit_message>
<xml_diff>
--- a/data/Diet and IBMR Conversions.xlsx
+++ b/data/Diet and IBMR Conversions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburdi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/synthesis coodination group/sdwsc/SDWSC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694D3413-F041-4A89-87F8-E96F491DC457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{67583272-9EF1-4B8C-855E-EE7D9676C803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02861C8C-B960-4D8E-958B-875A56F4E19F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BA0F259E-D3DF-404E-ADEB-41DD0350C243}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{BA0F259E-D3DF-404E-ADEB-41DD0350C243}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,10 +419,10 @@
     <t>shrimp</t>
   </si>
   <si>
+    <t>SHRIMP</t>
+  </si>
+  <si>
     <t>eurytem</t>
-  </si>
-  <si>
-    <t>sino</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -522,6 +522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,19 +860,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{410EBAF6-5D27-4DBD-871B-81D01562BE26}">
   <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
@@ -882,18 +883,18 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <v>3.36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -904,7 +905,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -915,29 +916,29 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>1.3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>79</v>
       </c>
@@ -948,29 +949,29 @@
         <v>2.98</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>2.67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9">
-        <v>1.1599999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -981,7 +982,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -992,7 +993,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>81</v>
       </c>
@@ -1003,7 +1004,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>82</v>
       </c>
@@ -1014,18 +1015,18 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -1036,7 +1037,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1047,7 +1048,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>84</v>
       </c>
@@ -1058,7 +1059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1069,7 +1070,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
@@ -1080,7 +1081,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>85</v>
       </c>
@@ -1091,7 +1092,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>123</v>
       </c>
@@ -1102,7 +1103,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
@@ -1113,7 +1114,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
@@ -1124,7 +1125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>86</v>
       </c>
@@ -1135,18 +1136,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -1157,7 +1158,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>88</v>
       </c>
@@ -1168,7 +1169,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
@@ -1179,7 +1180,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
@@ -1190,7 +1191,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
@@ -1201,29 +1202,29 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="6">
         <v>3.36</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>16</v>
       </c>
@@ -1234,7 +1235,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>92</v>
       </c>
@@ -1245,18 +1246,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="6">
         <v>1.5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>94</v>
       </c>
@@ -1267,18 +1268,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="6">
         <v>3.3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>17</v>
       </c>
@@ -1289,7 +1290,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>18</v>
       </c>
@@ -1300,29 +1301,29 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C40">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>97</v>
       </c>
@@ -1333,7 +1334,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>124</v>
       </c>
@@ -1344,7 +1345,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>20</v>
       </c>
@@ -1355,7 +1356,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>21</v>
       </c>
@@ -1366,7 +1367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>22</v>
       </c>
@@ -1377,7 +1378,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>23</v>
       </c>
@@ -1388,40 +1389,40 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="6">
         <v>0.04</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="6">
         <v>0.04</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="6">
         <v>0.13</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>25</v>
       </c>
@@ -1443,7 +1444,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>26</v>
       </c>
@@ -1454,7 +1455,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>27</v>
       </c>
@@ -1465,40 +1466,40 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C55">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C56">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="6">
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>102</v>
       </c>
@@ -1509,18 +1510,18 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>31</v>
       </c>
@@ -1531,18 +1532,18 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>33</v>
       </c>
@@ -1553,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>103</v>
       </c>
@@ -1564,7 +1565,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>34</v>
       </c>
@@ -1575,7 +1576,7 @@
         <v>3.36</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>104</v>
       </c>
@@ -1586,7 +1587,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>35</v>
       </c>
@@ -1597,7 +1598,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>36</v>
       </c>
@@ -1608,7 +1609,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>37</v>
       </c>
@@ -1619,7 +1620,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>105</v>
       </c>
@@ -1630,7 +1631,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>38</v>
       </c>
@@ -1641,18 +1642,18 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="6">
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>106</v>
       </c>
@@ -1663,40 +1664,40 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="6">
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="6">
         <v>2.66</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="6">
         <v>2.66</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>43</v>
       </c>
@@ -1707,7 +1708,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>44</v>
       </c>
@@ -1718,51 +1719,51 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="6">
         <v>2.66</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C79">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C80">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B79" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C79">
+      <c r="B81" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C81" s="6">
         <v>3.41</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C80">
-        <v>1.81</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C81">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>47</v>
       </c>
@@ -1773,7 +1774,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
         <v>48</v>
       </c>
@@ -1784,7 +1785,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>109</v>
       </c>
@@ -1795,18 +1796,18 @@
         <v>70</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="6">
         <v>0.12</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>50</v>
       </c>
@@ -1817,7 +1818,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>51</v>
       </c>
@@ -1828,7 +1829,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>110</v>
       </c>
@@ -1839,7 +1840,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>52</v>
       </c>
@@ -1850,18 +1851,18 @@
         <v>7.95</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="6">
         <v>15.89</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>54</v>
       </c>
@@ -1872,7 +1873,7 @@
         <v>15.89</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>111</v>
       </c>
@@ -1883,18 +1884,18 @@
         <v>15.89</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="6">
         <v>0.12</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>112</v>
       </c>
@@ -1905,7 +1906,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
         <v>113</v>
       </c>
@@ -1916,7 +1917,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>114</v>
       </c>
@@ -1927,7 +1928,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>115</v>
       </c>
@@ -1938,29 +1939,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>117</v>
       </c>
@@ -1971,7 +1972,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
         <v>118</v>
       </c>
@@ -1982,7 +1983,7 @@
         <v>3.36</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>57</v>
       </c>
@@ -1993,7 +1994,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>119</v>
       </c>
@@ -2004,7 +2005,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>120</v>
       </c>
@@ -2015,7 +2016,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>121</v>
       </c>
@@ -2026,18 +2027,18 @@
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C106">
+      <c r="C106" s="6">
         <v>0.1</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>122</v>
       </c>
@@ -2048,7 +2049,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>59</v>
       </c>
@@ -2060,6 +2061,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C108">
+    <sortCondition ref="A2:A108"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>